<commit_message>
Documentation added for all but QuickSort.py
</commit_message>
<xml_diff>
--- a/running_times.xlsx
+++ b/running_times.xlsx
@@ -467,34 +467,34 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>986.3376617431641</v>
+        <v>1994.132995605469</v>
       </c>
       <c r="C3">
-        <v>2007.007598876953</v>
+        <v>3989.934921264648</v>
       </c>
       <c r="D3">
-        <v>3989.219665527344</v>
+        <v>6980.89599609375</v>
       </c>
       <c r="E3">
-        <v>5018.472671508789</v>
+        <v>9972.572326660156</v>
       </c>
       <c r="F3">
-        <v>7978.439331054688</v>
+        <v>12964.24865722656</v>
       </c>
       <c r="G3">
-        <v>9973.526000976562</v>
+        <v>15957.35549926758</v>
       </c>
       <c r="H3">
-        <v>11967.65899658203</v>
+        <v>19946.81358337402</v>
       </c>
       <c r="I3">
-        <v>13973.23608398438</v>
+        <v>22938.48991394043</v>
       </c>
       <c r="J3">
-        <v>16954.18357849121</v>
+        <v>25896.78764343262</v>
       </c>
       <c r="K3">
-        <v>19954.91981506348</v>
+        <v>30897.37892150879</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -502,34 +502,34 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1989.841461181641</v>
+        <v>2992.153167724609</v>
       </c>
       <c r="C4">
-        <v>2989.053726196289</v>
+        <v>4987.955093383789</v>
       </c>
       <c r="D4">
-        <v>3989.219665527344</v>
+        <v>6981.611251831055</v>
       </c>
       <c r="E4">
-        <v>5983.114242553711</v>
+        <v>8976.459503173828</v>
       </c>
       <c r="F4">
-        <v>6981.372833251953</v>
+        <v>11968.37425231934</v>
       </c>
       <c r="G4">
-        <v>7978.200912475586</v>
+        <v>15959.02442932129</v>
       </c>
       <c r="H4">
-        <v>10970.5924987793</v>
+        <v>16954.42199707031</v>
       </c>
       <c r="I4">
-        <v>11962.4137878418</v>
+        <v>19947.05200195312</v>
       </c>
       <c r="J4">
-        <v>13962.5072479248</v>
+        <v>23962.97454833984</v>
       </c>
       <c r="K4">
-        <v>18940.68717956543</v>
+        <v>25928.97415161133</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -537,34 +537,34 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1991.748809814453</v>
+        <v>2991.914749145508</v>
       </c>
       <c r="C5">
-        <v>3991.842269897461</v>
+        <v>6980.419158935547</v>
       </c>
       <c r="D5">
-        <v>6982.088088989258</v>
+        <v>11969.32792663574</v>
       </c>
       <c r="E5">
-        <v>8986.473083496094</v>
+        <v>16954.18357849121</v>
       </c>
       <c r="F5">
-        <v>11968.13583374023</v>
+        <v>20943.88008117676</v>
       </c>
       <c r="G5">
-        <v>15986.44256591797</v>
+        <v>25929.92782592773</v>
       </c>
       <c r="H5">
-        <v>18949.98550415039</v>
+        <v>30917.16766357422</v>
       </c>
       <c r="I5">
-        <v>20946.02584838867</v>
+        <v>35904.4075012207</v>
       </c>
       <c r="J5">
-        <v>26927.70957946777</v>
+        <v>39864.77851867676</v>
       </c>
       <c r="K5">
-        <v>31951.4274597168</v>
+        <v>45877.45666503906</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -572,34 +572,34 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>15958.07075500488</v>
+        <v>27925.01449584961</v>
       </c>
       <c r="C6">
-        <v>64785.95733642578</v>
+        <v>115660.4290008545</v>
       </c>
       <c r="D6">
-        <v>152630.3291320801</v>
+        <v>250365.7341003418</v>
       </c>
       <c r="E6">
-        <v>261303.186416626</v>
+        <v>449797.3918914795</v>
       </c>
       <c r="F6">
-        <v>410901.7848968506</v>
+        <v>701125.8602142334</v>
       </c>
       <c r="G6">
-        <v>588397.2644805908</v>
+        <v>1031243.085861206</v>
       </c>
       <c r="H6">
-        <v>844741.8212890625</v>
+        <v>1378316.402435303</v>
       </c>
       <c r="I6">
-        <v>1092082.262039185</v>
+        <v>1795199.632644653</v>
       </c>
       <c r="J6">
-        <v>1404246.56867981</v>
+        <v>2350753.545761108</v>
       </c>
       <c r="K6">
-        <v>1700446.605682373</v>
+        <v>2811478.137969971</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -607,34 +607,34 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>14976.73988342285</v>
+        <v>43919.80171203613</v>
       </c>
       <c r="C7">
-        <v>62831.64024353027</v>
+        <v>151596.5461730957</v>
       </c>
       <c r="D7">
-        <v>141625.1659393311</v>
+        <v>360000.8487701416</v>
       </c>
       <c r="E7">
-        <v>258265.2568817139</v>
+        <v>666218.2807922363</v>
       </c>
       <c r="F7">
-        <v>397936.5825653076</v>
+        <v>998328.4473419189</v>
       </c>
       <c r="G7">
-        <v>581446.1708068848</v>
+        <v>1890941.858291626</v>
       </c>
       <c r="H7">
-        <v>806882.8582763672</v>
+        <v>2160223.245620728</v>
       </c>
       <c r="I7">
-        <v>1054140.090942383</v>
+        <v>2740709.066390991</v>
       </c>
       <c r="J7">
-        <v>1412221.670150757</v>
+        <v>3216392.278671265</v>
       </c>
       <c r="K7">
-        <v>1646610.498428345</v>
+        <v>3729995.012283325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>